<commit_message>
Download and ui fix
</commit_message>
<xml_diff>
--- a/server/expense_details.xlsx
+++ b/server/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,29 +416,172 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>dinner</v>
+        <v>Dal bati</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>45817.54185799768</v>
+        <v>45825.54185799768</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>fghj</v>
+      </c>
+      <c r="B3">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45825.00011574074</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>tttt</v>
+      </c>
+      <c r="B4">
+        <v>4444444</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45825.00011574074</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>dfghj</v>
+      </c>
+      <c r="B5">
+        <v>122222</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45825.00011574074</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Dal bati</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45824.54185799768</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>poiuyt</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45824.00011574074</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>dinner</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
         <v>lunch</v>
       </c>
-      <c r="B3">
+      <c r="B9">
         <v>500</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C9" s="1">
         <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>lunch</v>
+      </c>
+      <c r="B10">
+        <v>500</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45817.54185799768</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>test</v>
+      </c>
+      <c r="B11">
+        <v>500</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45816.54185799768</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>test</v>
+      </c>
+      <c r="B12">
+        <v>5000</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45814.54185799768</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>djhbf</v>
+      </c>
+      <c r="B13">
+        <v>5000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45813.54185799768</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>dfghjk</v>
+      </c>
+      <c r="B14">
+        <v>567777</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45811.00011574074</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>djhbf</v>
+      </c>
+      <c r="B15">
+        <v>5000</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45810.54185799768</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>toffee</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45809.54185799768</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>